<commit_message>
init translation landing-page and faq
</commit_message>
<xml_diff>
--- a/update_assets/input.xlsx
+++ b/update_assets/input.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadav\Documents\ALL_PROJECTS\smapy\update_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BDD552-A678-4B8E-A83B-D8B5ED30C2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A4C160-5095-409F-A5ED-0FFAC77C61F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44880" yWindow="-6825" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="101">
   <si>
     <t>key</t>
   </si>
@@ -182,117 +169,106 @@
     <t>index.sections.7.header</t>
   </si>
   <si>
-    <t xml:space="preserve"> קודבל ואוב
-!ונלש חוטיבה יריחמ תא</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> םלתשמה חוטיבה תא םכל הגישמ יפאמס
-!קודב הז ,רתויב</t>
-  </si>
-  <si>
-    <t>םייח חוטיב</t>
-  </si>
-  <si>
-    <t>השיכרו האוושהל</t>
-  </si>
-  <si>
-    <t>התנכשמ חוטיב</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> הריד חוטיב</t>
-  </si>
-  <si>
-    <t>פלטפורמת הביטוח המתקדמת ביותר  בישראל</t>
-  </si>
-  <si>
-    <t xml:space="preserve">םיישונא םיסנניפו חוטיב יחמומו היגולונכט תבלשמה תינשדח חוטיב תמרופטלפ איה Smapy </t>
-  </si>
-  <si>
-    <t>.דחא קילקב רתויב םלתשמהו ןוכנה חוטיבה תא שוכרל םכל רוזעתש ,AI תססובמ המרופטלפ
-  ןוכדע תועצמאב דימת רתויב בוטה חוטיבה תא םכל היהיש גאדתש ,תונשדחו תופיקשמ ונהת Smapy - ב
-.חוטיבה תויולעב םילקש יפלא תואמ דעו רקי ןמז ךוסחל ולכותש ךכ ,יטמוטוא ןפואב םכלש םיישיאה םיטרפהו הסילופה</t>
-  </si>
-  <si>
-    <t>דבוע הז ךיא</t>
-  </si>
-  <si>
-    <t>תורכיה</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> תא םכרובע רתאל לכונש ידכ
- וכרטצת ,רתויב תובוטה תועצהה
- רחא דימו ,םיטרפ 'סמ אלמל
- שופיחב םיליחתמ ונא ךכ
-.רתויב תמלתשמה העצהה</t>
-  </si>
-  <si>
-    <t>תועצה תלבק</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> תועצה תא םכל גיצת Smapy
- תומלתשמהו תובוטה חוטיבה
- םכל רוזעתו םכרובע רתויב
- המכח הרוצב חוטיב שוכרל
-.דיתעב תועתפה ענמתש</t>
-  </si>
-  <si>
-    <t>השיכר</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> הבוטה העצהב ורחבתש ירחא
- תא תונקל ולכות ,רתויב
- 'קד 5 -ב ןייל ןוא חוטיבה
- שאר יבאכ ןומה ךוסחלו
-.רקי ןמזו</t>
+    <t>index.sections.7.text</t>
+  </si>
+  <si>
+    <t>faq.header</t>
+  </si>
+  <si>
+    <t>faq.text</t>
+  </si>
+  <si>
+    <t>faq.questions.header</t>
+  </si>
+  <si>
+    <t>faq.contact.header</t>
+  </si>
+  <si>
+    <t>faq.contact.text</t>
+  </si>
+  <si>
+    <t>בואו לבדוק את מחירי הביטוח שלנו!</t>
+  </si>
+  <si>
+    <t>סמאפי משיגה לכם את הביטוח המשתלם ביותר, זה בדוק!</t>
+  </si>
+  <si>
+    <t>ביטוח חיים</t>
+  </si>
+  <si>
+    <t>ביטוח משכנתה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ביטוח דירה </t>
+  </si>
+  <si>
+    <t>להשוואה ורכישה</t>
+  </si>
+  <si>
+    <t>פלטפורמת הביטוח המתקדמת ביותר בישראל</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Smapy היא פלטפורמת ביטוח חדשנית המשלבת טכנולוגיה ומומחי ביטוח ופיננסים אנושיים</t>
+  </si>
+  <si>
+    <t>פלטפורמה מבוססת AI, שתעזור לכם לרכוש את הביטוח הנכון והמשתלם ביותר בקליק אחד. ב - Smapy תהנו משקיפות וחדשנות, שתדאג שיהיה לכם את הביטוח הטוב ביותר תמיד באמצעות עדכון הפוליסה והפרטים האישיים שלכם באופן אוטומטי, כך שתוכלו לחסוך זמן יקר ועד מאות אלפי שקלים בעלויות הביטוח.</t>
+  </si>
+  <si>
+    <t>איך זה עובד</t>
+  </si>
+  <si>
+    <t>היכרות</t>
+  </si>
+  <si>
+    <t>כדי שנוכל לאתר עבורכם את ההצעות הטובות ביותר, תצטרכו למלא מס' פרטים, ומיד אחר כך אנו מתחילים בחיפוש ההצעה המשתלמת ביותר.</t>
+  </si>
+  <si>
+    <t>קבלת הצעות</t>
+  </si>
+  <si>
+    <t>Smapy תציג לכם את הצעות הביטוח הטובות והמשתלמות ביותר עבורכם ותעזור לכם לרכוש ביטוח בצורה חכמה שתמנע הפתעות בעתיד.</t>
+  </si>
+  <si>
+    <t>רכישה</t>
+  </si>
+  <si>
+    <t>אחרי שתבחרו בהצעה הטובה ביותר, תוכלו לקנות את הביטוח און ליין ב- 5 דק' ולחסוך המון כאבי ראש וזמן יקר.</t>
   </si>
   <si>
     <t>איתכם לאורך כל הדרך</t>
   </si>
   <si>
-    <t xml:space="preserve">.טקש שארב תויהל ולכות וישכעמ
- ירחא בקעמב היהת יפאמס
- לכ ךרואל םכלש חוטיבה
- םכתא ןכדעל גאדתו וייח
-.דימת רתויב תמלתשמה העצהב </t>
-  </si>
-  <si>
-    <t>ךריחבל תורבח ןווגמ</t>
-  </si>
-  <si>
-    <t>-ב רוחבל תוביס עברא'</t>
+    <t>מעכשיו תוכלו להיות בראש שקט. סמאפי תהיה במעקב אחרי הביטוח שלכם לאורך כל חייו ותדאג לעדכן אתכם בהצעה המשתלמת ביותר תמיד.</t>
+  </si>
+  <si>
+    <t>מגוון חברות לבחירך</t>
+  </si>
+  <si>
+    <t>ארבע סיבות לבחור ב-</t>
   </si>
   <si>
     <t>ביטוח מותאם אישית</t>
   </si>
   <si>
-    <t>םיעדוי ונא ,ונחתיפש היגולונכטה תרזעב
-בוטהו ןוכנה חוטיבה תא םכל םיאתהל
-םכלש םיישיאה םינותנל םאותה ,רתויב
-.דיל הפפכ ומכ שממ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">הפוקש םיריחמ תאוושה </t>
-  </si>
-  <si>
-    <t>חוטיבה תורבחמ םילבקמ ונאש הלמעה זוחא
-תועצה תא םילבקמ םתא ןכלו ןלוכ ןיב ההז
-.סרטניא םוש אללו רתויב תובוטה ריחמה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ישפנ טקשו תונשדח </t>
-  </si>
-  <si>
-    <t>חוטיבה יאנתו ריחמ ירחא בקוע ונלש םתירוגלאה
-תיטמוטוא םיריחמ תאוושה עצבמו םכלש
-.היהתש רתויב הבוטה העצהל ןוכדעו</t>
-  </si>
-  <si>
-    <t>בוט םישוע</t>
-  </si>
-  <si>
-    <t>ונלש חוורהמ קלח םימרות ונא חוטיב תשיכר לכב
-רשאכ םידבוע ונא םתיא םינוגראהמ דחאל
-.ונובשח לע אלו חוקלה םשב היהת המורתה</t>
+    <t>בעזרת הטכנולוגיה שפיתחנו, אנו יודעים להתאים לכם את הביטוח הנכון והטוב ביותר, התואם לנתונים האישיים שלכם ממש כמו כפפה ליד.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> השוואת מחירים שקופה</t>
+  </si>
+  <si>
+    <t>אחוז העמלה שאנו מקבלים מחברות הביטוח זהה בין כולן ולכן אתם מקבלים את הצעות המחיר הטובות ביותר וללא שום אינטרס.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> חדשנות ושקט נפשי</t>
+  </si>
+  <si>
+    <t>האלגוריתם שלנו עוקב אחרי מחיר ותנאי הביטוח שלכם ומבצע השוואת מחירים אוטומטית ועדכון להצעה הטובה ביותר שתהיה.</t>
+  </si>
+  <si>
+    <t>עושים טוב</t>
+  </si>
+  <si>
+    <t>בכל רכישת ביטוח אנו תורמים חלק מהרווח שלנו לאחד מהארגונים איתם אנו עובדים כאשר התרומה תהיה בשם הלקוח ולא על חשבונו.</t>
   </si>
   <si>
     <t>מה אומרים עלינו</t>
@@ -328,10 +304,25 @@
     <t>מה יקרה מיד לאחר התשלום?</t>
   </si>
   <si>
-    <t>&lt; תופסונ תולאשל</t>
-  </si>
-  <si>
-    <t>!רוזעל חמשנ</t>
+    <t>לשאלות נוספות &gt;</t>
+  </si>
+  <si>
+    <t>נשמח לעזור!</t>
+  </si>
+  <si>
+    <t>בכל דרך שתבחרו..</t>
+  </si>
+  <si>
+    <t>שאלות ותשובות נפוצות</t>
+  </si>
+  <si>
+    <t>רתויב תוצופנה תולאשה תא םכרובע ונזכיר ?רורב אל והשמ</t>
+  </si>
+  <si>
+    <t>צריכים מידע נוסף?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> אנו זמינים לכל שאלה או בקשה!</t>
   </si>
 </sst>
 </file>
@@ -349,7 +340,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -393,15 +387,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -463,7 +453,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,9 +485,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -529,6 +537,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -705,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,26 +750,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>49</v>
+      <c r="B2" t="s">
+        <v>55</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>50</v>
+      <c r="B3" t="s">
+        <v>56</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,10 +777,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,10 +788,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,10 +799,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -784,10 +810,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -795,30 +821,32 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>57</v>
+      <c r="B10" t="s">
+        <v>63</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,10 +854,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,21 +865,21 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>60</v>
+      <c r="B13" t="s">
+        <v>66</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,21 +887,21 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>62</v>
+      <c r="B15" t="s">
+        <v>68</v>
       </c>
       <c r="C15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,21 +909,21 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>64</v>
+      <c r="B17" t="s">
+        <v>70</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -903,19 +931,21 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>66</v>
+      <c r="B19" t="s">
+        <v>72</v>
       </c>
       <c r="C19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,21 +953,21 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>68</v>
+      <c r="B21" t="s">
+        <v>74</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,19 +975,21 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>70</v>
+      <c r="B23" t="s">
+        <v>76</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -965,21 +997,21 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>72</v>
+      <c r="B25" t="s">
+        <v>78</v>
       </c>
       <c r="C25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,21 +1019,21 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>74</v>
+      <c r="B27" t="s">
+        <v>80</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,21 +1041,21 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="270" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>76</v>
+      <c r="B29" t="s">
+        <v>82</v>
       </c>
       <c r="C29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,19 +1063,21 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1051,10 +1085,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1062,10 +1096,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1073,10 +1107,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1084,10 +1118,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1095,10 +1129,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1106,10 +1140,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1117,10 +1151,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1128,18 +1162,22 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1149,7 +1187,7 @@
         <v>42</v>
       </c>
       <c r="C41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,9 +1195,11 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1169,7 +1209,7 @@
         <v>44</v>
       </c>
       <c r="C43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,9 +1217,11 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1189,7 +1231,7 @@
         <v>46</v>
       </c>
       <c r="C45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1197,10 +1239,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,13 +1250,79 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="2">
         <v>1</v>
       </c>
     </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update_he.py console log updated| landing - page updated
</commit_message>
<xml_diff>
--- a/update_assets/input.xlsx
+++ b/update_assets/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadav\Documents\ALL_PROJECTS\smapy\update_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4396C045-A81E-4F60-8A25-BCF023F4BAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D6875C-AB55-4E03-B4D5-7BA6C843A44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-6825" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>key</t>
   </si>
@@ -31,135 +31,52 @@
     <t>format_flag</t>
   </si>
   <si>
-    <t>about.header</t>
-  </si>
-  <si>
-    <t>about.buy</t>
-  </si>
-  <si>
-    <t>about.tech.header</t>
-  </si>
-  <si>
-    <t>about.tech.text</t>
-  </si>
-  <si>
-    <t>about.vision.header</t>
-  </si>
-  <si>
-    <t>about.vision.header_2</t>
-  </si>
-  <si>
-    <t>about.vision.text</t>
-  </si>
-  <si>
-    <t>about.profile.1.name</t>
-  </si>
-  <si>
-    <t>about.profile.1.role_en</t>
-  </si>
-  <si>
-    <t>about.profile.1.role_he</t>
-  </si>
-  <si>
-    <t>about.profile.1.text</t>
-  </si>
-  <si>
-    <t>about.profile.2.name</t>
-  </si>
-  <si>
-    <t>about.profile.2.role_en</t>
-  </si>
-  <si>
-    <t>about.profile.2.role_he</t>
-  </si>
-  <si>
-    <t>about.profile.2.text</t>
-  </si>
-  <si>
-    <t>about.profile.3.name</t>
-  </si>
-  <si>
-    <t>about.profile.3.role_en</t>
-  </si>
-  <si>
-    <t>about.profile.3.role_he</t>
-  </si>
-  <si>
-    <t>about.profile.3.text</t>
-  </si>
-  <si>
-    <t>about.about_us.header</t>
-  </si>
-  <si>
-    <t>קליק אחד ותוכלו לחסוך עד עשרות אלפי שקלים בביטוח.</t>
-  </si>
-  <si>
-    <t>חוטיב תשיכרל</t>
-  </si>
-  <si>
-    <t>טכנולוגיה, חדשנות ושקיפות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">לשמחת כולנו, אנו חיים בעידן בו הטכנולוגיה יוצאת מן הכלל ועוזרת למין האנושי באינספור תחומים כדי להפוך את החיים לטובים יותר.
-מהיום, גם בביטוחים שלכם, סמאפי תוכל לבצע לכם אופטימיזציה באמצעות טכנולוגיה ייחודית שפיתחנו, ובכך לחסוך לכם כאבי ראש,
-זמן יקר והמון כסף, תוך כדי שקיפות מלאה, פשטות וחווית שירות שטרם הכרתם. רוב האנשים נאלצים לסמוך על מה שנציגי המכירות 
-אומרים להם, אבל עם Smapy זה אחרת - סמאפי מציגה לכם את הצעות הביטוח המשתלמות ביותר ותמליץ לכם על הביטוח הטוב ביותר.
-איך אנחנו עושים זאת? פשוט מאוד, יצרנו מודל עסקי מול חברות הביטוח בו אנו מקבלים עמלה אחידה וזהה, כך אנו יכולים להבטיח לכם 
-שההצעות וההמלצות שתקבלו מאיתנו הן שקופות, אובייקטיביות ונטולות אינטרס. 
-סמאפי מחפשת את ההצעות הטובות ביותר בין חברות הביטוח ובין עשרות מסלולים שהן מציעות עד שאתם מקבלים את ההצעה המשתלמת
-ביותר. אם תמצאו הצעה טובה יותר – תקבלו מאיתנו שירות ללא כל עלות! חשוב לציין שלצד הטכנולוגיה, תוכלו לקבל שירות ממומחי
- ביטוח ופיננסים שישמחו לעזור ולתת לכם את המענה הטוב ביותר לכל שאלה או בקשה. </t>
-  </si>
-  <si>
-    <t>החזון של סמאפי</t>
-  </si>
-  <si>
-    <t>לשנות את עולם הביטוח לפשוט, שקוף ומשתלם לכולם!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ונלגיד לע ונטרח .תחאו דחא לכל ,רתויב לוזהו בוטה חוטיבה תשיכרל רתויב בוטה ןורתפה תויהל ידכ המקוה יפאמס
- ,ורובע רתויב לוזהו בוטה חוטיבה תא לבקל ליג לכב םדא לכל רשפאל ידכ תורישהו תונשדחה ,תופיקשה אשונ תא
-תיברימ תוחונו תופיקש ,תוטשפב לכה .חוטיב הלימה תא עמושש סאבתהל וא ,השתה תמחלמ רובעל ךרטציש ילבמ
-.םכרובע רתויב בוטה ןורתפה תויהל ונל םירשפאמ ,ישונאה יווילה םע דחי ,ונחתיפש היגולונכטה תועצמאב תאזו </t>
-  </si>
-  <si>
-    <t>זבלא ןדרו'ג</t>
-  </si>
-  <si>
-    <t>יקסלש ליג</t>
-  </si>
-  <si>
-    <t>דבוע לאומש ילומ</t>
-  </si>
-  <si>
-    <t>Co-Founder &amp; CEO</t>
-  </si>
-  <si>
-    <t>מייסד ומנכ’’ל משותף</t>
-  </si>
-  <si>
-    <t>יזם, מומחה בתכנון פיננסי, פנסיוני וניהול סיכונים. בעל רישיון ממשרד האוצר, מנהל הון, ביטוח וחסכונות למאות משפחות בישראל. מעל 10 שנות ניסיון בביטוח, חסכון ושוק ההון. בוגר קורסים בתחום משכנתאות, נדל''ן, שוק ההון פנסיה וביטוח.</t>
-  </si>
-  <si>
-    <t>Chairman and founder Co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מייסד ויושב ראש </t>
-  </si>
-  <si>
-    <t>מומחה בביטוח חיים וביטוח פנסיוני. כיהן במגוון תפקידי ניהול בכירים בחברות הביטוח הגדולות במשק. מתמחה בבניית מוצרי ביטוח לחברות הגדולות במשק.</t>
-  </si>
-  <si>
-    <t>Co-Founder &amp; CTO</t>
-  </si>
-  <si>
-    <t>מייסד וסמנכ’’ל טכנולוגיות.</t>
-  </si>
-  <si>
-    <t>יזם, מנהל פיתוח וארכיטרקט  תוכנה, מעל 20 שנות ניסיון בניהול ופיתוח טכנולוגיות, הקים וניהל קבוצות פיתוח והוביל פיתוח מוצרים מורכבים במספר חברות.</t>
-  </si>
-  <si>
-    <t>מי אנחנו</t>
+    <t>index.sections.6.faqs.1.a</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.2.q</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.2.a</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.3.q</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.3.a</t>
+  </si>
+  <si>
+    <t>index.sections.6.more_faqs</t>
+  </si>
+  <si>
+    <t>index.sections.7.header</t>
+  </si>
+  <si>
+    <t>index.sections.7.text</t>
+  </si>
+  <si>
+    <t>האם ההשוואה נעשית מול כל חברות הביטוח?</t>
+  </si>
+  <si>
+    <t>מה יקרה מיד לאחר התשלום?</t>
+  </si>
+  <si>
+    <t>לשאלות נוספות &gt;</t>
+  </si>
+  <si>
+    <t>נשמח לעזור!</t>
+  </si>
+  <si>
+    <t>בכל דרך שתבחרו..</t>
+  </si>
+  <si>
+    <t>כן! סמאפי מבצעת השוואת מחירים מול כל חברות הביטוח הגדולות (הראל, פניקס, מגדל, איילון, כלל, הכשרה ומנורה) בהתאם לפרופיל הלקוח ולתנאי הביטוח שצריך. ההשוואה מתבצעת בין כל החברות וגם בין עשרות המסלולים שכל חברה מציע ומציגה את התוצאות הטובות ביותר שהתקבלו.</t>
+  </si>
+  <si>
+    <t>כן! ההשוואה נעשית בדרך כלל מול שבע חברות ביטוח ומציגה את ההצעות הזולות ביותר בהתאם לביטוח הדרוש ולפרופיל שלך כלקוח.</t>
+  </si>
+  <si>
+    <t>מיד לאחר התשלום, תקבל מייל עם אישור רכישת הביטוח. במידה ואין כל בעיה רפואית, תקבל גם את פוליסת הביטוח שלך. בנוסף, ישלח לך קישור לאזור האישי שלך, בו תוכל להתעדכן בסטטוס רכישת הביטוח. לדו'ג אם חברת הביטוח תצטרך ממך מסמך כלשהו, תוכל לראות זאת באיזור האישי וגם נעדכן במייל ובהודעת וואטסאפ לנוחיות מירבית. בנוסף לכל זה, סמאפי ממנה מומחה ביטוח שידאג להיות איתך בקשר לכל שאלה או בקשה.</t>
   </si>
 </sst>
 </file>
@@ -183,18 +100,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -224,14 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,9 +502,9 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2">
+        <v>16</v>
+      </c>
+      <c r="C2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -606,10 +513,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -617,20 +524,20 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -639,9 +546,9 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2">
+        <v>18</v>
+      </c>
+      <c r="C6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -650,21 +557,21 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -672,141 +579,9 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="C9" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed common.json, moved nav translation to landing-page.json
</commit_message>
<xml_diff>
--- a/update_assets/input.xlsx
+++ b/update_assets/input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="202">
   <si>
     <t>key</t>
   </si>
@@ -25,25 +25,304 @@
     <t>format_flag</t>
   </si>
   <si>
-    <t>dangerous_hobby_validation</t>
-  </si>
-  <si>
-    <t>property_apartment_number_validation</t>
-  </si>
-  <si>
-    <t>property_city_validation</t>
-  </si>
-  <si>
-    <t>property_street_number_validation</t>
-  </si>
-  <si>
-    <t>property_street_validation</t>
-  </si>
-  <si>
-    <t>smoking_stop_month_validation</t>
-  </si>
-  <si>
-    <t>wizard.end.button</t>
+    <t>index.header</t>
+  </si>
+  <si>
+    <t>index.header_2</t>
+  </si>
+  <si>
+    <t>index.floating.1</t>
+  </si>
+  <si>
+    <t>index.floating.2</t>
+  </si>
+  <si>
+    <t>index.floating.3</t>
+  </si>
+  <si>
+    <t>index.floating.link_text</t>
+  </si>
+  <si>
+    <t>index.sections.1.header</t>
+  </si>
+  <si>
+    <t>index.sections.1.text.1</t>
+  </si>
+  <si>
+    <t>index.sections.1.text.2</t>
+  </si>
+  <si>
+    <t>index.sections.2.header</t>
+  </si>
+  <si>
+    <t>index.sections.2.steps.1.title</t>
+  </si>
+  <si>
+    <t>index.sections.2.steps.1.text</t>
+  </si>
+  <si>
+    <t>index.sections.2.steps.2.title</t>
+  </si>
+  <si>
+    <t>index.sections.2.steps.2.text</t>
+  </si>
+  <si>
+    <t>index.sections.2.steps.3.title</t>
+  </si>
+  <si>
+    <t>index.sections.2.steps.3.text</t>
+  </si>
+  <si>
+    <t>index.sections.2.steps.4.title</t>
+  </si>
+  <si>
+    <t>index.sections.2.steps.4.text</t>
+  </si>
+  <si>
+    <t>index.sections.3.header</t>
+  </si>
+  <si>
+    <t>index.sections.4.header</t>
+  </si>
+  <si>
+    <t>index.sections.4.reasons.1.title</t>
+  </si>
+  <si>
+    <t>index.sections.4.reasons.1.text</t>
+  </si>
+  <si>
+    <t>index.sections.4.reasons.2.title</t>
+  </si>
+  <si>
+    <t>index.sections.4.reasons.2.text</t>
+  </si>
+  <si>
+    <t>index.sections.4.reasons.3.title</t>
+  </si>
+  <si>
+    <t>index.sections.4.reasons.3.text</t>
+  </si>
+  <si>
+    <t>index.sections.4.reasons.4.title</t>
+  </si>
+  <si>
+    <t>index.sections.4.reasons.4.text</t>
+  </si>
+  <si>
+    <t>index.sections.5.header</t>
+  </si>
+  <si>
+    <t>index.sections.5.cards.1.name</t>
+  </si>
+  <si>
+    <t>index.sections.5.cards.1.text</t>
+  </si>
+  <si>
+    <t>index.sections.5.cards.2.name</t>
+  </si>
+  <si>
+    <t>index.sections.5.cards.2.text</t>
+  </si>
+  <si>
+    <t>index.sections.5.cards.3.name</t>
+  </si>
+  <si>
+    <t>index.sections.5.cards.3.text</t>
+  </si>
+  <si>
+    <t>index.sections.5.cards.4.name</t>
+  </si>
+  <si>
+    <t>index.sections.5.cards.4.text</t>
+  </si>
+  <si>
+    <t>index.sections.6.header</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.1.q</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.1.a</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.2.q</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.2.a</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.3.q</t>
+  </si>
+  <si>
+    <t>index.sections.6.faqs.3.a</t>
+  </si>
+  <si>
+    <t>index.sections.6.more_faqs</t>
+  </si>
+  <si>
+    <t>index.sections.7.header</t>
+  </si>
+  <si>
+    <t>index.sections.7.text</t>
+  </si>
+  <si>
+    <t>faq.header</t>
+  </si>
+  <si>
+    <t>faq.text</t>
+  </si>
+  <si>
+    <t>faq.questions.header</t>
+  </si>
+  <si>
+    <t>faq.contact.header</t>
+  </si>
+  <si>
+    <t>faq.contact.text</t>
+  </si>
+  <si>
+    <t>about.header</t>
+  </si>
+  <si>
+    <t>about.buy</t>
+  </si>
+  <si>
+    <t>about.tech.header</t>
+  </si>
+  <si>
+    <t>about.tech.text</t>
+  </si>
+  <si>
+    <t>about.vision.header</t>
+  </si>
+  <si>
+    <t>about.vision.header_2</t>
+  </si>
+  <si>
+    <t>about.vision.text</t>
+  </si>
+  <si>
+    <t>about.profile.1.name</t>
+  </si>
+  <si>
+    <t>about.profile.1.role_en</t>
+  </si>
+  <si>
+    <t>about.profile.1.role_he</t>
+  </si>
+  <si>
+    <t>about.profile.1.text</t>
+  </si>
+  <si>
+    <t>about.profile.2.name</t>
+  </si>
+  <si>
+    <t>about.profile.2.role_en</t>
+  </si>
+  <si>
+    <t>about.profile.2.role_he</t>
+  </si>
+  <si>
+    <t>about.profile.2.text</t>
+  </si>
+  <si>
+    <t>about.profile.3.name</t>
+  </si>
+  <si>
+    <t>about.profile.3.role_en</t>
+  </si>
+  <si>
+    <t>about.profile.3.role_he</t>
+  </si>
+  <si>
+    <t>about.profile.3.text</t>
+  </si>
+  <si>
+    <t>about.about_us.header</t>
+  </si>
+  <si>
+    <t>price.0.1</t>
+  </si>
+  <si>
+    <t>price.0.2</t>
+  </si>
+  <si>
+    <t>price.0.3</t>
+  </si>
+  <si>
+    <t>price.0.4</t>
+  </si>
+  <si>
+    <t>price.0.5</t>
+  </si>
+  <si>
+    <t>price.1.name</t>
+  </si>
+  <si>
+    <t>price.1.price</t>
+  </si>
+  <si>
+    <t>price.2.name</t>
+  </si>
+  <si>
+    <t>price.2.price</t>
+  </si>
+  <si>
+    <t>price.3.name</t>
+  </si>
+  <si>
+    <t>price.3.price</t>
+  </si>
+  <si>
+    <t>price.3.extra_line</t>
+  </si>
+  <si>
+    <t>price.header</t>
+  </si>
+  <si>
+    <t>price.text</t>
+  </si>
+  <si>
+    <t>price.header2</t>
+  </si>
+  <si>
+    <t>price.cost</t>
+  </si>
+  <si>
+    <t>price.cost_service</t>
+  </si>
+  <si>
+    <t>price.free</t>
+  </si>
+  <si>
+    <t>price.footer</t>
+  </si>
+  <si>
+    <t>price.footer2</t>
+  </si>
+  <si>
+    <t>security.header</t>
+  </si>
+  <si>
+    <t>security.text</t>
+  </si>
+  <si>
+    <t>security.header2</t>
+  </si>
+  <si>
+    <t>security.text1</t>
+  </si>
+  <si>
+    <t>security.text2</t>
+  </si>
+  <si>
+    <t>security.logo.1</t>
+  </si>
+  <si>
+    <t>security.logo.2</t>
+  </si>
+  <si>
+    <t>security.logo.3</t>
   </si>
   <si>
     <t>nav.about</t>
@@ -64,28 +343,283 @@
     <t>nav.agent_entry</t>
   </si>
   <si>
-    <t>*TRANSLATE*</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
-    <t>קצת עלינו</t>
+    <t>בואו לבדוק את מחירי הביטוח שלנו!</t>
+  </si>
+  <si>
+    <t>סמאפי משיגה לכם את הביטוח המשתלם ביותר, זה בדוק!</t>
+  </si>
+  <si>
+    <t>ביטוח חיים</t>
+  </si>
+  <si>
+    <t>ביטוח משכנתה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ביטוח דירה </t>
+  </si>
+  <si>
+    <t>להשוואה ורכישה</t>
+  </si>
+  <si>
+    <t>פלטפורמת הביטוח המתקדמת ביותר בישראל</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Smapy היא פלטפורמת ביטוח חדשנית המשלבת טכנולוגיה ומומחי ביטוח ופיננסים אנושיים</t>
+  </si>
+  <si>
+    <t>פלטפורמה מבוססת AI, שתעזור לכם לרכוש את הביטוח הנכון והמשתלם ביותר בקליק אחד. ב - Smapy תהנו משקיפות וחדשנות, שתדאג שיהיה לכם את הביטוח הטוב ביותר תמיד באמצעות עדכון הפוליסה והפרטים האישיים שלכם באופן אוטומטי, כך שתוכלו לחסוך זמן יקר ועד מאות אלפי שקלים בעלויות הביטוח.</t>
+  </si>
+  <si>
+    <t>איך זה עובד</t>
+  </si>
+  <si>
+    <t>היכרות</t>
+  </si>
+  <si>
+    <t>כדי שנוכל לאתר עבורכם את ההצעות הטובות ביותר, תצטרכו למלא מס' פרטים, ומיד אחר כך אנו מתחילים בחיפוש ההצעה המשתלמת ביותר.</t>
+  </si>
+  <si>
+    <t>קבלת הצעות</t>
+  </si>
+  <si>
+    <t>Smapy תציג לכם את הצעות הביטוח הטובות והמשתלמות ביותר עבורכם ותעזור לכם לרכוש ביטוח בצורה חכמה שתמנע הפתעות בעתיד.</t>
+  </si>
+  <si>
+    <t>רכישה</t>
+  </si>
+  <si>
+    <t>אחרי שתבחרו בהצעה הטובה ביותר, תוכלו לקנות את הביטוח און ליין ב- 5 דק' ולחסוך המון כאבי ראש וזמן יקר.</t>
+  </si>
+  <si>
+    <t>איתכם לאורך כל הדרך</t>
+  </si>
+  <si>
+    <t>מעכשיו תוכלו להיות בראש שקט. סמאפי תהיה במעקב אחרי הביטוח שלכם לאורך כל חייו ותדאג לעדכן אתכם בהצעה המשתלמת ביותר תמיד.</t>
+  </si>
+  <si>
+    <t>מגוון חברות לבחירך</t>
+  </si>
+  <si>
+    <t>ארבע סיבות לבחור ב-</t>
+  </si>
+  <si>
+    <t>ביטוח מותאם אישית</t>
+  </si>
+  <si>
+    <t>בעזרת הטכנולוגיה שפיתחנו, אנו יודעים להתאים לכם את הביטוח הנכון והטוב ביותר, התואם לנתונים האישיים שלכם ממש כמו כפפה ליד.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> השוואת מחירים שקופה</t>
+  </si>
+  <si>
+    <t>אחוז העמלה שאנו מקבלים מחברות הביטוח זהה בין כולן ולכן אתם מקבלים את הצעות המחיר הטובות ביותר וללא שום אינטרס.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> חדשנות ושקט נפשי</t>
+  </si>
+  <si>
+    <t>האלגוריתם שלנו עוקב אחרי מחיר ותנאי הביטוח שלכם ומבצע השוואת מחירים אוטומטית ועדכון להצעה הטובה ביותר שתהיה.</t>
+  </si>
+  <si>
+    <t>עושים טוב</t>
+  </si>
+  <si>
+    <t>בכל רכישת ביטוח אנו תורמים חלק מהרווח שלנו לאחד מהארגונים איתם אנו עובדים כאשר התרומה תהיה בשם הלקוח ולא על חשבונו.</t>
+  </si>
+  <si>
+    <t>מה אומרים עלינו</t>
+  </si>
+  <si>
+    <t>Ms. Tony Rutherford</t>
+  </si>
+  <si>
+    <t>Everyone’s on the same page. Many of our people are not very organized naturally, so Pharps is a godsend!</t>
+  </si>
+  <si>
+    <t>Agnes Lockman</t>
+  </si>
+  <si>
+    <t>If you are a business owner, and you don't have Xalor in your toolkit just yet, I highly recommend that you check it out.</t>
+  </si>
+  <si>
+    <t>Hugo Nienow</t>
+  </si>
+  <si>
+    <t>I have been using this software for over a year now and I love it! I can't imagine life without it. It's so easy to use, and the customer service is great.</t>
   </si>
   <si>
     <t>שאלות נפוצות</t>
   </si>
   <si>
+    <t>האם סמאפי עובדת עם כל חברות הביטוח?</t>
+  </si>
+  <si>
+    <t>כן! סמאפי מבצעת השוואת מחירים מול כל חברות הביטוח הגדולות (הראל, פניקס, מגדל, איילון, כלל, הכשרה ומנורה) בהתאם לפרופיל הלקוח ולתנאי הביטוח שצריך. ההשוואה מתבצעת בין כל החברות וגם בין עשרות המסלולים שכל חברה מציע ומציגה את התוצאות הטובות ביותר שהתקבלו.</t>
+  </si>
+  <si>
+    <t>האם ההשוואה נעשית מול כל חברות הביטוח?</t>
+  </si>
+  <si>
+    <t>כן! ההשוואה נעשית בדרך כלל מול שבע חברות ביטוח ומציגה את ההצעות הזולות ביותר בהתאם לביטוח הדרוש ולפרופיל שלך כלקוח.</t>
+  </si>
+  <si>
+    <t>מה יקרה מיד לאחר התשלום?</t>
+  </si>
+  <si>
+    <t>מיד לאחר התשלום, תקבל מייל עם אישור רכישת הביטוח. במידה ואין כל בעיה רפואית, תקבל גם את פוליסת הביטוח שלך. בנוסף, ישלח לך קישור לאזור האישי שלך, בו תוכל להתעדכן בסטטוס רכישת הביטוח. לדו'ג אם חברת הביטוח תצטרך ממך מסמך כלשהו, תוכל לראות זאת באיזור האישי וגם נעדכן במייל ובהודעת וואטסאפ לנוחיות מירבית. בנוסף לכל זה, סמאפי ממנה מומחה ביטוח שידאג להיות איתך בקשר לכל שאלה או בקשה.</t>
+  </si>
+  <si>
+    <t>לשאלות נוספות &gt;</t>
+  </si>
+  <si>
+    <t>נשמח לעזור!</t>
+  </si>
+  <si>
+    <t>בכל דרך שתבחרו..</t>
+  </si>
+  <si>
+    <t>שאלות ותשובות נפוצות</t>
+  </si>
+  <si>
+    <t>משהו לא ברור? ריכזנו עבורכם את השאלות הנפוצות ביותר</t>
+  </si>
+  <si>
+    <t>צריכים מידע נוסף?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> אנו זמינים לכל שאלה או בקשה!</t>
+  </si>
+  <si>
+    <t>קליק אחד ותוכלו לחסוך עד עשרות אלפי שקלים בביטוח.</t>
+  </si>
+  <si>
+    <t>לרכישת ביטוח</t>
+  </si>
+  <si>
+    <t>טכנולוגיה, חדשנות ושקיפות</t>
+  </si>
+  <si>
+    <t xml:space="preserve">לשמחת כולנו, אנו חיים בעידן בו הטכנולוגיה יוצאת מן הכלל ועוזרת למין האנושי באינספור תחומים כדי להפוך את החיים לטובים יותר. מהיום, גם בביטוחים שלכם, סמאפי תוכל לבצע לכם אופטימיזציה באמצעות טכנולוגיה ייחודית שפיתחנו, ובכך לחסוך לכם כאבי ראש, זמן יקר והמון כסף, תוך כדי שקיפות מלאה, פשטות וחווית שירות שטרם הכרתם. רוב האנשים נאלצים לסמוך על מה שנציגי המכירות אומרים להם, אבל עם Smapy זה אחרת - סמאפי מציגה לכם את הצעות הביטוח המשתלמות ביותר ותמליץ לכם על הביטוח הטוב ביותר. איך אנחנו עושים זאת? פשוט מאוד, יצרנו מודל עסקי מול חברות הביטוח בו אנו מקבלים עמלה אחידה וזהה, כך אנו יכולים להבטיח לכם שההצעות וההמלצות שתקבלו מאיתנו הן שקופות, אובייקטיביות ונטולות אינטרס. סמאפי מחפשת את ההצעות הטובות ביותר בין חברות הביטוח ובין עשרות מסלולים שהן מציעות עד שאתם מקבלים את ההצעה המשתלמת ביותר. אם תמצאו הצעה טובה יותר – תקבלו מאיתנו שירות ללא כל עלות! חשוב לציין שלצד הטכנולוגיה, תוכלו לקבל שירות ממומחי ביטוח ופיננסים שישמחו לעזור ולתת לכם את המענה הטוב ביותר לכל שאלה או בקשה. </t>
+  </si>
+  <si>
+    <t>החזון של סמאפי</t>
+  </si>
+  <si>
+    <t>לשנות את עולם הביטוח לפשוט, שקוף ומשתלם לכולם!</t>
+  </si>
+  <si>
+    <t>סמאפי הוקמה כדי להיות הפתרון הטוב ביותר לרכישת הביטוח הטוב והזול ביותר, לכל אחד ואחת. חרטנו על דיגלנו את נושא השקיפות, החדשנות והשירות כדי לאפשר לכל אדם בכל גיל לקבל את הביטוח הטוב והזול ביותר עבורו, מבלי שיצטרך לעבור מלחמת התשה, או להתבאס ששומע את המילה ביטוח. הכל בפשטות, שקיפות ונוחות מירבית וזאת באמצעות הטכנולוגיה שפיתחנו, יחד עם הליווי האנושי, מאפשרים לנו להיות הפתרון הטוב ביותר עבורכם.</t>
+  </si>
+  <si>
+    <t>ג'ורדן אלבז</t>
+  </si>
+  <si>
+    <t>Co-Founder &amp; CEO</t>
+  </si>
+  <si>
+    <t>מייסד ומנכ’’ל משותף</t>
+  </si>
+  <si>
+    <t>יזם, מומחה בתכנון פיננסי, פנסיוני וניהול סיכונים. בעל רישיון ממשרד האוצר, מנהל הון, ביטוח וחסכונות למאות משפחות בישראל. מעל 10 שנות ניסיון בביטוח, חסכון ושוק ההון. בוגר קורסים בתחום משכנתאות, נדל''ן, שוק ההון פנסיה וביטוח.</t>
+  </si>
+  <si>
+    <t>גיל שלסקי</t>
+  </si>
+  <si>
+    <t>Chairman and founder Co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מייסד ויושב ראש </t>
+  </si>
+  <si>
+    <t>מומחה בביטוח חיים וביטוח פנסיוני. כיהן במגוון תפקידי ניהול בכירים בחברות הביטוח הגדולות במשק. מתמחה בבניית מוצרי ביטוח לחברות הגדולות במשק.</t>
+  </si>
+  <si>
+    <t>מולי שמואל עובד</t>
+  </si>
+  <si>
+    <t>Co-Founder &amp; CTO</t>
+  </si>
+  <si>
+    <t>מייסד וסמנכ’’ל טכנולוגיות.</t>
+  </si>
+  <si>
+    <t>יזם, מנהל פיתוח וארכיטרקט תוכנה, מעל 20 שנות ניסיון בניהול ופיתוח טכנולוגיות, הקים וניהל קבוצות פיתוח והוביל פיתוח מוצרים מורכבים במספר חברות.</t>
+  </si>
+  <si>
+    <t>מי אנחנו</t>
+  </si>
+  <si>
+    <t>השוואה בין כל חברות הביטוח</t>
+  </si>
+  <si>
+    <t>ההצעות המשתלמות ביותר</t>
+  </si>
+  <si>
+    <t>המלצה על רכישת ביטוח בצורה חכמה</t>
+  </si>
+  <si>
+    <t>השוואת ביטוח קיים להצעה טובה יותר</t>
+  </si>
+  <si>
+    <t>מעקב אחרי מחיר ותנאי הביטוח לתמיד</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ביטוח חיים למשכנתה </t>
+  </si>
+  <si>
+    <t>החל מ- 10 ₪ לחודש</t>
+  </si>
+  <si>
+    <t>ביטוח מבנה למשכנתה</t>
+  </si>
+  <si>
+    <t>החל מ- 30 ₪ לחודש</t>
+  </si>
+  <si>
+    <t>ביטוח חיים למשפחה</t>
+  </si>
+  <si>
+    <t>החל מ- 7 ₪ לחודש</t>
+  </si>
+  <si>
+    <t>התאמת הביטוח לסטטוס האישי והכלכלי</t>
+  </si>
+  <si>
+    <t>המחיר זול, השירות יוקרתי</t>
+  </si>
+  <si>
+    <t>מגוון ביטוחים לכל שלב בחיים שיחסכו לכם כמויות של כסף</t>
+  </si>
+  <si>
     <t>מחירון</t>
   </si>
   <si>
+    <t>עלות הביטוח</t>
+  </si>
+  <si>
+    <t>עלות השירות</t>
+  </si>
+  <si>
+    <t>חינם</t>
+  </si>
+  <si>
+    <t>מצאתם הצעה טובה יותר? קבלו מאיתנו שירות מעקב אחרי הביטוח ללא עלות!</t>
+  </si>
+  <si>
+    <t>בהתאם למדיניות השירות באתר</t>
+  </si>
+  <si>
+    <t>הפרטיות שלכם היא הכל בשבילנו.</t>
+  </si>
+  <si>
     <t>אבטחה ופרטיות</t>
   </si>
   <si>
-    <t>כניסת לקוחות</t>
-  </si>
-  <si>
-    <t>כניסת יועצים/סוכנים</t>
+    <t xml:space="preserve">אבטחת מידע הוא אחד מהנושאים החשובים ביותר ברכישה און ליין, בטח שמדובר במידע אישי כמו ביטוח ופיננסים, אנחנו בסמאפי עושים הכל כדי לשמור על המידע הפרטי הזה ומחוייבים לא לעשות בו שום שימוש ולא להעביר אותו לאף צד שלישי שלא במסגרת השירות. עם סמאפי אתם יכולים להיות בטוחים ורגועים. </t>
+  </si>
+  <si>
+    <t>[img] גאה להיות מפוקחת על ידי רגולטורים פיננסים: בנק ישראל, רשות שוק ההון, ביטוח וחיסכון והרשות לניירות ערך. לפי הוראותיהם, כל המידע הפיננסי מוצפן ומופרד באופן הרמטי ממערכות עובדי החברה, כך שרק לכם ולמערכת הטכנולוגית יש גישה אליו. אף אחד מאיתנו לא יכול לגשת למידע בלי אישורכם!</t>
   </si>
 </sst>
 </file>
@@ -443,7 +977,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,7 +999,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>109</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -476,7 +1010,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -487,7 +1021,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -498,7 +1032,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -509,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -520,7 +1054,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -531,7 +1065,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -542,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -553,7 +1087,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -564,7 +1098,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -575,7 +1109,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -586,7 +1120,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -597,9 +1131,1032 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="b">
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
+        <v>161</v>
+      </c>
+      <c r="C57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" t="s">
+        <v>166</v>
+      </c>
+      <c r="C62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" t="s">
+        <v>169</v>
+      </c>
+      <c r="C65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" t="s">
+        <v>171</v>
+      </c>
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" t="s">
+        <v>174</v>
+      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" t="s">
+        <v>175</v>
+      </c>
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" t="s">
+        <v>178</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" t="s">
+        <v>179</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" t="s">
+        <v>181</v>
+      </c>
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" t="s">
+        <v>183</v>
+      </c>
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" t="s">
+        <v>184</v>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" t="s">
+        <v>185</v>
+      </c>
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" t="s">
+        <v>187</v>
+      </c>
+      <c r="C83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" t="s">
+        <v>188</v>
+      </c>
+      <c r="C84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" t="s">
+        <v>189</v>
+      </c>
+      <c r="C85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>190</v>
+      </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" t="s">
+        <v>191</v>
+      </c>
+      <c r="C87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>192</v>
+      </c>
+      <c r="C88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>194</v>
+      </c>
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" t="s">
+        <v>195</v>
+      </c>
+      <c r="C91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" t="s">
+        <v>196</v>
+      </c>
+      <c r="C92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" t="s">
+        <v>197</v>
+      </c>
+      <c r="C93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" t="s">
+        <v>198</v>
+      </c>
+      <c r="C94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" t="s">
+        <v>96</v>
+      </c>
+      <c r="C95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" t="s">
+        <v>199</v>
+      </c>
+      <c r="C96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" t="s">
+        <v>200</v>
+      </c>
+      <c r="C97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98" t="s">
+        <v>201</v>
+      </c>
+      <c r="C98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>102</v>
+      </c>
+      <c r="B101" t="s">
+        <v>102</v>
+      </c>
+      <c r="C101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>103</v>
+      </c>
+      <c r="B102" t="s">
+        <v>103</v>
+      </c>
+      <c r="C102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103" t="s">
+        <v>104</v>
+      </c>
+      <c r="C103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104" t="s">
+        <v>105</v>
+      </c>
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>107</v>
+      </c>
+      <c r="B106" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" t="s">
+        <v>108</v>
+      </c>
+      <c r="C107" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
translated customer & advisors entry
</commit_message>
<xml_diff>
--- a/update_assets/input.xlsx
+++ b/update_assets/input.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadav\Documents\ALL_PROJECTS\smapy\update_assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415A01B1-7D2A-4277-AAFA-4F20C5242904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-6825" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="215">
   <si>
     <t>key</t>
   </si>
@@ -343,6 +349,21 @@
     <t>nav.agent_entry</t>
   </si>
   <si>
+    <t>login.label</t>
+  </si>
+  <si>
+    <t>login.entry_customer</t>
+  </si>
+  <si>
+    <t>login.entry_advisor</t>
+  </si>
+  <si>
+    <t>login.id_card_number.label</t>
+  </si>
+  <si>
+    <t>login.phone.label</t>
+  </si>
+  <si>
     <t>בואו לבדוק את מחירי הביטוח שלנו!</t>
   </si>
   <si>
@@ -620,13 +641,37 @@
   </si>
   <si>
     <t>[img] גאה להיות מפוקחת על ידי רגולטורים פיננסים: בנק ישראל, רשות שוק ההון, ביטוח וחיסכון והרשות לניירות ערך. לפי הוראותיהם, כל המידע הפיננסי מוצפן ומופרד באופן הרמטי ממערכות עובדי החברה, כך שרק לכם ולמערכת הטכנולוגית יש גישה אליו. אף אחד מאיתנו לא יכול לגשת למידע בלי אישורכם!</t>
+  </si>
+  <si>
+    <t>קצת עלינו</t>
+  </si>
+  <si>
+    <t>כניסת לקוחות</t>
+  </si>
+  <si>
+    <t>כניסת יועצים/סוכנים</t>
+  </si>
+  <si>
+    <t>תוחוקל תסינכ</t>
+  </si>
+  <si>
+    <t>!בוש ךתוארל םיחמש</t>
+  </si>
+  <si>
+    <t>תוהז תדועת</t>
+  </si>
+  <si>
+    <t>ןופלט רפסמ</t>
+  </si>
+  <si>
+    <t>םינכוס/םיצעוי תסינכ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,6 +734,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -735,7 +788,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -767,9 +820,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -801,6 +872,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -976,14 +1065,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C107"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,1030 +1085,1030 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C88" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C89" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C90" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C91" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C92" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C93" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C94" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -2028,40 +2119,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C96" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C97" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C98" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -2072,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>101</v>
       </c>
@@ -2083,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -2094,70 +2185,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>103</v>
+        <v>207</v>
       </c>
       <c r="C102" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="C103" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>105</v>
+        <v>197</v>
       </c>
       <c r="C104" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="C105" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="C106" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>108</v>
+        <v>209</v>
       </c>
       <c r="C107" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108" t="s">
+        <v>211</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
+      <c r="B109" t="s">
+        <v>210</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>111</v>
+      </c>
+      <c r="B110" t="s">
+        <v>214</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111" t="s">
+        <v>212</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>113</v>
+      </c>
+      <c r="B112" t="s">
+        <v>213</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
translated 'next' buttons and otp text
</commit_message>
<xml_diff>
--- a/update_assets/input.xlsx
+++ b/update_assets/input.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadav\Documents\ALL_PROJECTS\smapy\update_assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9D98BD-D5F3-43A7-A023-9CE29D0F50D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="5280" yWindow="3030" windowWidth="16410" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="235">
   <si>
     <t>key</t>
   </si>
@@ -376,12 +382,24 @@
     <t>otp.pin.label</t>
   </si>
   <si>
+    <t>otp.next</t>
+  </si>
+  <si>
     <t>Token has expired or is invalid</t>
   </si>
   <si>
     <t>Not valid israeli id number</t>
   </si>
   <si>
+    <t>String must contain at least 6 character(s)</t>
+  </si>
+  <si>
+    <t>Not a valid phone number</t>
+  </si>
+  <si>
+    <t>user_id.next</t>
+  </si>
+  <si>
     <t>בואו לבדוק את מחירי הביטוח שלנו!</t>
   </si>
   <si>
@@ -679,7 +697,10 @@
     <t>מספר טלפון</t>
   </si>
   <si>
-    <t>Confirmation and continue</t>
+    <t>שדה חובה</t>
+  </si>
+  <si>
+    <t>אימות קטן וממשיכים..</t>
   </si>
   <si>
     <t>Sent you confirmation code in SMS message</t>
@@ -688,17 +709,29 @@
     <t>Customer entry</t>
   </si>
   <si>
-    <t>Advisor entry</t>
-  </si>
-  <si>
-    <t>What is your code</t>
+    <t>כניסת יועצים/ות</t>
+  </si>
+  <si>
+    <t>מהו הקוד שקיבלת?</t>
+  </si>
+  <si>
+    <t>המשך</t>
+  </si>
+  <si>
+    <t>קוד אימות שגוי או לא בתוקף</t>
+  </si>
+  <si>
+    <t>מספר זהות בלתי חוקי</t>
+  </si>
+  <si>
+    <t>מספר טלפון בלתי חוקי</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,6 +794,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -807,7 +848,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -839,9 +880,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -873,6 +932,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1048,14 +1125,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C120"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1066,1030 +1145,1030 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C88" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C89" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C90" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C91" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C92" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C93" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C94" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -2100,40 +2179,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C96" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C97" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C98" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -2144,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>101</v>
       </c>
@@ -2155,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -2166,212 +2245,256 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C102" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C103" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C104" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C105" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C106" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C107" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C108" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C109" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C110" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C111" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C112" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>114</v>
+        <v>225</v>
       </c>
       <c r="C113" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C114" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C115" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C116" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C117" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C118" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>120</v>
+        <v>231</v>
       </c>
       <c r="C119" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>121</v>
+        <v>232</v>
       </c>
       <c r="C120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>122</v>
+      </c>
+      <c r="B121" t="s">
+        <v>233</v>
+      </c>
+      <c r="C121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>123</v>
+      </c>
+      <c r="B122" t="s">
+        <v>123</v>
+      </c>
+      <c r="C122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>125</v>
+      </c>
+      <c r="B124" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>